<commit_message>
registration fix: all tables created properly
</commit_message>
<xml_diff>
--- a/app/static/user_data/logins.xlsx
+++ b/app/static/user_data/logins.xlsx
@@ -25,10 +25,10 @@
     <t>Сергеевич</t>
   </si>
   <si>
-    <t>stashevskiy.a.s.2016</t>
-  </si>
-  <si>
-    <t>pN7iSL54</t>
+    <t>stashevskiy.a.s.2017</t>
+  </si>
+  <si>
+    <t>vnlCts78</t>
   </si>
   <si>
     <t>Трубицын</t>
@@ -40,10 +40,10 @@
     <t>Алексеевич</t>
   </si>
   <si>
-    <t>trubicin.yu.a.2016</t>
-  </si>
-  <si>
-    <t>cnfnHlfC</t>
+    <t>trubicin.yu.a.2017</t>
+  </si>
+  <si>
+    <t>9wvEF7OT</t>
   </si>
   <si>
     <t>Смирнов</t>
@@ -55,10 +55,10 @@
     <t>Викторович</t>
   </si>
   <si>
-    <t>smirnov.s.v.2016</t>
-  </si>
-  <si>
-    <t>roGhGEqE</t>
+    <t>smirnov.s.v.2017</t>
+  </si>
+  <si>
+    <t>8DMIhIyK</t>
   </si>
   <si>
     <t>Горохов</t>
@@ -67,10 +67,10 @@
     <t>Никита</t>
   </si>
   <si>
-    <t>gorohov.n.s.2016</t>
-  </si>
-  <si>
-    <t>VXtrwVO1</t>
+    <t>gorohov.n.s.2017</t>
+  </si>
+  <si>
+    <t>QSG3Yn89</t>
   </si>
   <si>
     <t>Южаков</t>
@@ -79,10 +79,10 @@
     <t>Тимофей</t>
   </si>
   <si>
-    <t>yujakov.t.a.2016</t>
-  </si>
-  <si>
-    <t>daXvFt81</t>
+    <t>yujakov.t.a.2017</t>
+  </si>
+  <si>
+    <t>X97yaHif</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
search changes, promps date, bugfixes
</commit_message>
<xml_diff>
--- a/app/static/user_data/logins.xlsx
+++ b/app/static/user_data/logins.xlsx
@@ -14,90 +14,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
-    <t>Сташевский</t>
+    <t>Фам</t>
   </si>
   <si>
-    <t>Андрей</t>
+    <t>Им</t>
   </si>
   <si>
-    <t>Сергеевич</t>
+    <t>Отч</t>
   </si>
   <si>
-    <t>stashevskiy.a.s.2222</t>
+    <t>fam.i.o.123</t>
   </si>
   <si>
-    <t>3kkP4etE</t>
-  </si>
-  <si>
-    <t>Трубицын</t>
-  </si>
-  <si>
-    <t>Юрий</t>
-  </si>
-  <si>
-    <t>Алексеевич</t>
-  </si>
-  <si>
-    <t>trubicin.yu.a.2222</t>
-  </si>
-  <si>
-    <t>L48uMtEy</t>
-  </si>
-  <si>
-    <t>Смирнов</t>
-  </si>
-  <si>
-    <t>Сергей</t>
-  </si>
-  <si>
-    <t>Викторович</t>
-  </si>
-  <si>
-    <t>smirnov.s.v.2222</t>
-  </si>
-  <si>
-    <t>VlTqyT1q</t>
-  </si>
-  <si>
-    <t>Горохов</t>
-  </si>
-  <si>
-    <t>Никита</t>
-  </si>
-  <si>
-    <t>gorohov.n.s.2222</t>
-  </si>
-  <si>
-    <t>WcThvF2P</t>
-  </si>
-  <si>
-    <t>Южаков</t>
-  </si>
-  <si>
-    <t>Тимофей</t>
-  </si>
-  <si>
-    <t>yujakov.t.a.2222</t>
-  </si>
-  <si>
-    <t>PH3fP6ke</t>
+    <t>oERJr1Hz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt formatCode="General" numFmtId="164"/>
+  </numFmts>
+  <fonts count="4">
     <font>
-      <name val="Calibri"/>
-      <charset val="204"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,16 +77,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium4" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -205,7 +177,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -240,7 +211,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -275,16 +245,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -406,72 +380,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="44" zoomScaleNormal="44" zoomScalePageLayoutView="100">
+      <selection activeCell="C2" activeCellId="0" pane="topLeft" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1025" min="1" width="11.5204081632653"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row customHeight="1" ht="12.8" r="1" s="1" spans="1:5">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -481,75 +419,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="1" usePrinterDefaults="0" verticalDpi="300"/>
+  <headerFooter differentFirst="0" differentOddEven="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>